<commit_message>
Array School Level Problems.....
</commit_message>
<xml_diff>
--- a/School_Level_Problems/Excel_Files/1_Arrays/School_Level_Array_Problems.xlsx
+++ b/School_Level_Problems/Excel_Files/1_Arrays/School_Level_Array_Problems.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
   <si>
     <t>SrNo</t>
   </si>
@@ -631,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -759,7 +759,9 @@
       <c r="D7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="5">
@@ -774,7 +776,9 @@
       <c r="D8" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5">
@@ -789,7 +793,9 @@
       <c r="D9" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="5">
@@ -804,7 +810,9 @@
       <c r="D10" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="5">
@@ -819,7 +827,9 @@
       <c r="D11" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="5">
@@ -834,7 +844,9 @@
       <c r="D12" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="5">
@@ -849,7 +861,9 @@
       <c r="D13" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="5">
@@ -864,7 +878,9 @@
       <c r="D14" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="5">
@@ -879,7 +895,9 @@
       <c r="D15" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="5">
@@ -894,7 +912,9 @@
       <c r="D16" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="5">
@@ -909,7 +929,9 @@
       <c r="D17" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="5">
@@ -924,7 +946,9 @@
       <c r="D18" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="5">
@@ -939,7 +963,9 @@
       <c r="D19" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="5">
@@ -954,7 +980,9 @@
       <c r="D20" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="5">
@@ -969,7 +997,9 @@
       <c r="D21" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="5">

</xml_diff>